<commit_message>
aded best model, noit yet tested
</commit_message>
<xml_diff>
--- a/Assignment 2/report/result_overview.xlsx
+++ b/Assignment 2/report/result_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richa\Documents\Programmieren\Deep-Learning-2022\Assignment 2\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DC3A75A-1F64-47B8-B0F6-BF464CF762EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F73578-543B-40D7-9C12-AF77F7B38A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{BCEC3F85-B862-4DC7-ADA0-7EF6B88461F9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="14">
   <si>
     <t>Adam</t>
   </si>
@@ -56,13 +56,37 @@
     <t>relu</t>
   </si>
   <si>
-    <t>ExponentialDecay</t>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Activation function</t>
+  </si>
+  <si>
+    <t>Validation Loss</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>SGD-Mom</t>
+  </si>
+  <si>
+    <t>Exp. dec.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,16 +116,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -112,6 +162,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AACC4186-4B82-428D-9829-96D3D4F3E141}" name="Tabelle1" displayName="Tabelle1" ref="B1:F37" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B1:F37" xr:uid="{AACC4186-4B82-428D-9829-96D3D4F3E141}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F37">
+    <sortCondition ref="F1:F37"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{9D6E47A4-2AD2-46AE-91B1-3403150994ED}" name="Optimizer" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{7D131B31-7050-4ED7-91A1-818D1D975044}" name="Structure" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{CD0E9BBA-2B84-4475-B8F0-112879157600}" name="Activation function" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{81873C0E-598E-4C92-A679-0661A1FF55AC}" name="Learning Rate" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{64342010-1B13-4FB9-BC0C-BF2F4FF7B5AD}" name="Validation Loss" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,33 +478,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C04A275-146B-45A4-834F-11BA0EE9460A}">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2.37800413742661E-3</v>
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.4270012034103201E-3</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
@@ -445,16 +532,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
         <v>1E-4</v>
       </c>
-      <c r="F3" s="1">
-        <v>1.6497421311214499E-3</v>
+      <c r="F3" s="2">
+        <v>1.5307973371818601E-3</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
@@ -467,11 +554,11 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1.6906958771869499E-3</v>
+      <c r="E4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.55478215310722E-3</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
@@ -479,16 +566,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1">
         <v>1E-4</v>
       </c>
-      <c r="F5" s="1">
-        <v>1.55478215310722E-3</v>
+      <c r="F5" s="2">
+        <v>1.5609047841280599E-3</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
@@ -496,16 +583,16 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1.9306868780404299E-3</v>
+        <v>13</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.60934915766119E-3</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
@@ -513,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
@@ -521,8 +608,8 @@
       <c r="E7" s="1">
         <v>1E-4</v>
       </c>
-      <c r="F7" s="1">
-        <v>1.5609047841280599E-3</v>
+      <c r="F7" s="2">
+        <v>1.6497421311214499E-3</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
@@ -530,16 +617,16 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1.8963566981255999E-3</v>
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.6873026033863399E-3</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
@@ -547,33 +634,33 @@
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1.5307973371818601E-3</v>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.6906958771869499E-3</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1.9023531349375801E-3</v>
+      <c r="E10" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.86150590889155E-3</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
@@ -581,16 +668,16 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1.6873026033863399E-3</v>
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.8963566981255999E-3</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
@@ -601,33 +688,468 @@
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1.60934915766119E-3</v>
+        <v>13</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.9023531349375801E-3</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1">
         <v>1E-4</v>
       </c>
-      <c r="F13" s="1">
-        <v>1.4270012034103201E-3</v>
+      <c r="F13" s="2">
+        <v>1.92233105190098E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.9306868780404299E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2.0066197030246201E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2.1306746639311301E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2.1689319983124698E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.2433702833950498E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2.37800413742661E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2.5474352296441698E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2.5815395638346598E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F22" s="2">
+        <v>3.1622236128896401E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F23" s="2">
+        <v>3.5286203492432798E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3.6166862118989199E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3.7825843319296802E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3.8518600631505199E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3.8971265312284201E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F28" s="2">
+        <v>4.35514654964208E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2">
+        <v>4.6051219105720503E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="2">
+        <v>6.9872615858912399E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7.3664374649524602E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="2">
+        <v>7.7293901704251697E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1.23966066166758E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.5979040414094901E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1.6202310100197698E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="2">
+        <v>3.3875882625579799E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="2">
+        <v>4.6001300215721103E-2</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:F25">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F37">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>